<commit_message>
Fix: Eliminada metadata (Company: Positiva) de plantilla Excel
</commit_message>
<xml_diff>
--- a/backend/app/services/plantilla_valoracion_simple.xlsx
+++ b/backend/app/services/plantilla_valoracion_simple.xlsx
@@ -75,7 +75,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -89,11 +89,39 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -112,6 +140,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -509,9 +539,6 @@
           <t>Fecha de valoración:</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
@@ -527,6 +554,13 @@
         </is>
       </c>
       <c r="B5" s="5" t="n"/>
+      <c r="C5" s="10" t="n"/>
+      <c r="D5" s="10" t="n"/>
+      <c r="E5" s="10" t="n"/>
+      <c r="F5" s="10" t="n"/>
+      <c r="G5" s="10" t="n"/>
+      <c r="H5" s="10" t="n"/>
+      <c r="I5" s="11" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
@@ -535,6 +569,13 @@
         </is>
       </c>
       <c r="B6" s="5" t="n"/>
+      <c r="C6" s="10" t="n"/>
+      <c r="D6" s="10" t="n"/>
+      <c r="E6" s="10" t="n"/>
+      <c r="F6" s="10" t="n"/>
+      <c r="G6" s="10" t="n"/>
+      <c r="H6" s="10" t="n"/>
+      <c r="I6" s="11" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
@@ -542,9 +583,6 @@
           <t>Fecha de nacimiento:</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
       <c r="F7" s="2" t="inlineStr">
         <is>
           <t>Edad:</t>
@@ -608,6 +646,13 @@
         </is>
       </c>
       <c r="B10" s="6" t="n"/>
+      <c r="C10" s="10" t="n"/>
+      <c r="D10" s="10" t="n"/>
+      <c r="E10" s="10" t="n"/>
+      <c r="F10" s="10" t="n"/>
+      <c r="G10" s="10" t="n"/>
+      <c r="H10" s="10" t="n"/>
+      <c r="I10" s="11" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
@@ -616,6 +661,13 @@
         </is>
       </c>
       <c r="B11" s="5" t="n"/>
+      <c r="C11" s="10" t="n"/>
+      <c r="D11" s="10" t="n"/>
+      <c r="E11" s="10" t="n"/>
+      <c r="F11" s="10" t="n"/>
+      <c r="G11" s="10" t="n"/>
+      <c r="H11" s="10" t="n"/>
+      <c r="I11" s="11" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="4" t="inlineStr">
@@ -624,6 +676,13 @@
         </is>
       </c>
       <c r="B12" s="5" t="n"/>
+      <c r="C12" s="10" t="n"/>
+      <c r="D12" s="10" t="n"/>
+      <c r="E12" s="10" t="n"/>
+      <c r="F12" s="10" t="n"/>
+      <c r="G12" s="10" t="n"/>
+      <c r="H12" s="10" t="n"/>
+      <c r="I12" s="11" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
@@ -632,6 +691,13 @@
         </is>
       </c>
       <c r="B13" s="5" t="n"/>
+      <c r="C13" s="10" t="n"/>
+      <c r="D13" s="10" t="n"/>
+      <c r="E13" s="10" t="n"/>
+      <c r="F13" s="10" t="n"/>
+      <c r="G13" s="10" t="n"/>
+      <c r="H13" s="10" t="n"/>
+      <c r="I13" s="11" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="4" t="inlineStr">
@@ -684,6 +750,13 @@
         </is>
       </c>
       <c r="B18" s="5" t="n"/>
+      <c r="C18" s="10" t="n"/>
+      <c r="D18" s="10" t="n"/>
+      <c r="E18" s="10" t="n"/>
+      <c r="F18" s="10" t="n"/>
+      <c r="G18" s="10" t="n"/>
+      <c r="H18" s="10" t="n"/>
+      <c r="I18" s="11" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
@@ -692,6 +765,13 @@
         </is>
       </c>
       <c r="B19" s="5" t="n"/>
+      <c r="C19" s="10" t="n"/>
+      <c r="D19" s="10" t="n"/>
+      <c r="E19" s="10" t="n"/>
+      <c r="F19" s="10" t="n"/>
+      <c r="G19" s="10" t="n"/>
+      <c r="H19" s="10" t="n"/>
+      <c r="I19" s="11" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
@@ -714,6 +794,13 @@
         </is>
       </c>
       <c r="B21" s="5" t="n"/>
+      <c r="C21" s="10" t="n"/>
+      <c r="D21" s="10" t="n"/>
+      <c r="E21" s="10" t="n"/>
+      <c r="F21" s="10" t="n"/>
+      <c r="G21" s="10" t="n"/>
+      <c r="H21" s="10" t="n"/>
+      <c r="I21" s="11" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
@@ -722,6 +809,13 @@
         </is>
       </c>
       <c r="B22" s="5" t="n"/>
+      <c r="C22" s="10" t="n"/>
+      <c r="D22" s="10" t="n"/>
+      <c r="E22" s="10" t="n"/>
+      <c r="F22" s="10" t="n"/>
+      <c r="G22" s="10" t="n"/>
+      <c r="H22" s="10" t="n"/>
+      <c r="I22" s="11" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="4" t="inlineStr">
@@ -744,6 +838,13 @@
         </is>
       </c>
       <c r="B24" s="5" t="n"/>
+      <c r="C24" s="10" t="n"/>
+      <c r="D24" s="10" t="n"/>
+      <c r="E24" s="10" t="n"/>
+      <c r="F24" s="10" t="n"/>
+      <c r="G24" s="10" t="n"/>
+      <c r="H24" s="10" t="n"/>
+      <c r="I24" s="11" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
@@ -763,34 +864,54 @@
           <t>Cargo/Funciones</t>
         </is>
       </c>
+      <c r="C27" s="10" t="n"/>
+      <c r="D27" s="11" t="n"/>
       <c r="E27" s="7" t="inlineStr">
         <is>
           <t>Duración</t>
         </is>
       </c>
+      <c r="F27" s="11" t="n"/>
       <c r="G27" s="7" t="inlineStr">
         <is>
           <t>Motivo de retiro</t>
         </is>
       </c>
+      <c r="H27" s="10" t="n"/>
+      <c r="I27" s="11" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="n"/>
       <c r="B28" s="5" t="n"/>
+      <c r="C28" s="10" t="n"/>
+      <c r="D28" s="11" t="n"/>
       <c r="E28" s="5" t="n"/>
+      <c r="F28" s="11" t="n"/>
       <c r="G28" s="5" t="n"/>
+      <c r="H28" s="10" t="n"/>
+      <c r="I28" s="11" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="n"/>
       <c r="B29" s="5" t="n"/>
+      <c r="C29" s="10" t="n"/>
+      <c r="D29" s="11" t="n"/>
       <c r="E29" s="5" t="n"/>
+      <c r="F29" s="11" t="n"/>
       <c r="G29" s="5" t="n"/>
+      <c r="H29" s="10" t="n"/>
+      <c r="I29" s="11" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="n"/>
       <c r="B30" s="5" t="n"/>
+      <c r="C30" s="10" t="n"/>
+      <c r="D30" s="11" t="n"/>
       <c r="E30" s="5" t="n"/>
+      <c r="F30" s="11" t="n"/>
       <c r="G30" s="5" t="n"/>
+      <c r="H30" s="10" t="n"/>
+      <c r="I30" s="11" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="4" t="inlineStr">
@@ -799,6 +920,13 @@
         </is>
       </c>
       <c r="B32" s="6" t="n"/>
+      <c r="C32" s="10" t="n"/>
+      <c r="D32" s="10" t="n"/>
+      <c r="E32" s="10" t="n"/>
+      <c r="F32" s="10" t="n"/>
+      <c r="G32" s="10" t="n"/>
+      <c r="H32" s="10" t="n"/>
+      <c r="I32" s="11" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="4" t="inlineStr">
@@ -807,6 +935,13 @@
         </is>
       </c>
       <c r="B33" s="6" t="n"/>
+      <c r="C33" s="10" t="n"/>
+      <c r="D33" s="10" t="n"/>
+      <c r="E33" s="10" t="n"/>
+      <c r="F33" s="10" t="n"/>
+      <c r="G33" s="10" t="n"/>
+      <c r="H33" s="10" t="n"/>
+      <c r="I33" s="11" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
@@ -822,6 +957,13 @@
         </is>
       </c>
       <c r="B36" s="5" t="n"/>
+      <c r="C36" s="10" t="n"/>
+      <c r="D36" s="10" t="n"/>
+      <c r="E36" s="10" t="n"/>
+      <c r="F36" s="10" t="n"/>
+      <c r="G36" s="10" t="n"/>
+      <c r="H36" s="10" t="n"/>
+      <c r="I36" s="11" t="n"/>
     </row>
     <row r="37" ht="30" customHeight="1">
       <c r="A37" s="4" t="inlineStr">
@@ -830,6 +972,13 @@
         </is>
       </c>
       <c r="B37" s="6" t="n"/>
+      <c r="C37" s="10" t="n"/>
+      <c r="D37" s="10" t="n"/>
+      <c r="E37" s="10" t="n"/>
+      <c r="F37" s="10" t="n"/>
+      <c r="G37" s="10" t="n"/>
+      <c r="H37" s="10" t="n"/>
+      <c r="I37" s="11" t="n"/>
     </row>
     <row r="38">
       <c r="A38" s="4" t="inlineStr">
@@ -838,6 +987,13 @@
         </is>
       </c>
       <c r="B38" s="6" t="n"/>
+      <c r="C38" s="10" t="n"/>
+      <c r="D38" s="10" t="n"/>
+      <c r="E38" s="10" t="n"/>
+      <c r="F38" s="10" t="n"/>
+      <c r="G38" s="10" t="n"/>
+      <c r="H38" s="10" t="n"/>
+      <c r="I38" s="11" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="4" t="inlineStr">
@@ -846,6 +1002,13 @@
         </is>
       </c>
       <c r="B39" s="5" t="n"/>
+      <c r="C39" s="10" t="n"/>
+      <c r="D39" s="10" t="n"/>
+      <c r="E39" s="10" t="n"/>
+      <c r="F39" s="10" t="n"/>
+      <c r="G39" s="10" t="n"/>
+      <c r="H39" s="10" t="n"/>
+      <c r="I39" s="11" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="4" t="inlineStr">
@@ -854,6 +1017,13 @@
         </is>
       </c>
       <c r="B40" s="6" t="n"/>
+      <c r="C40" s="10" t="n"/>
+      <c r="D40" s="10" t="n"/>
+      <c r="E40" s="10" t="n"/>
+      <c r="F40" s="10" t="n"/>
+      <c r="G40" s="10" t="n"/>
+      <c r="H40" s="10" t="n"/>
+      <c r="I40" s="11" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
@@ -868,6 +1038,11 @@
           <t>Factor de Riesgo</t>
         </is>
       </c>
+      <c r="B43" s="10" t="n"/>
+      <c r="C43" s="10" t="n"/>
+      <c r="D43" s="10" t="n"/>
+      <c r="E43" s="10" t="n"/>
+      <c r="F43" s="11" t="n"/>
       <c r="G43" s="8" t="inlineStr">
         <is>
           <t>SI</t>
@@ -890,6 +1065,14 @@
           <t>DEMANDAS CUANTITATIVAS</t>
         </is>
       </c>
+      <c r="B44" s="10" t="n"/>
+      <c r="C44" s="10" t="n"/>
+      <c r="D44" s="10" t="n"/>
+      <c r="E44" s="10" t="n"/>
+      <c r="F44" s="10" t="n"/>
+      <c r="G44" s="10" t="n"/>
+      <c r="H44" s="10" t="n"/>
+      <c r="I44" s="11" t="n"/>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="6" t="inlineStr">
@@ -897,6 +1080,11 @@
           <t xml:space="preserve">   Item 1</t>
         </is>
       </c>
+      <c r="B45" s="10" t="n"/>
+      <c r="C45" s="10" t="n"/>
+      <c r="D45" s="10" t="n"/>
+      <c r="E45" s="10" t="n"/>
+      <c r="F45" s="11" t="n"/>
       <c r="G45" s="5" t="n"/>
       <c r="H45" s="5" t="n"/>
       <c r="I45" s="5" t="n"/>
@@ -907,6 +1095,11 @@
           <t xml:space="preserve">   Item 2</t>
         </is>
       </c>
+      <c r="B46" s="10" t="n"/>
+      <c r="C46" s="10" t="n"/>
+      <c r="D46" s="10" t="n"/>
+      <c r="E46" s="10" t="n"/>
+      <c r="F46" s="11" t="n"/>
       <c r="G46" s="5" t="n"/>
       <c r="H46" s="5" t="n"/>
       <c r="I46" s="5" t="n"/>
@@ -917,6 +1110,11 @@
           <t xml:space="preserve">   Item 3</t>
         </is>
       </c>
+      <c r="B47" s="10" t="n"/>
+      <c r="C47" s="10" t="n"/>
+      <c r="D47" s="10" t="n"/>
+      <c r="E47" s="10" t="n"/>
+      <c r="F47" s="11" t="n"/>
       <c r="G47" s="5" t="n"/>
       <c r="H47" s="5" t="n"/>
       <c r="I47" s="5" t="n"/>
@@ -927,6 +1125,11 @@
           <t xml:space="preserve">   Item 4</t>
         </is>
       </c>
+      <c r="B48" s="10" t="n"/>
+      <c r="C48" s="10" t="n"/>
+      <c r="D48" s="10" t="n"/>
+      <c r="E48" s="10" t="n"/>
+      <c r="F48" s="11" t="n"/>
       <c r="G48" s="5" t="n"/>
       <c r="H48" s="5" t="n"/>
       <c r="I48" s="5" t="n"/>
@@ -937,6 +1140,14 @@
           <t>DEMANDAS DE CARGA MENTAL</t>
         </is>
       </c>
+      <c r="B49" s="10" t="n"/>
+      <c r="C49" s="10" t="n"/>
+      <c r="D49" s="10" t="n"/>
+      <c r="E49" s="10" t="n"/>
+      <c r="F49" s="10" t="n"/>
+      <c r="G49" s="10" t="n"/>
+      <c r="H49" s="10" t="n"/>
+      <c r="I49" s="11" t="n"/>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="6" t="inlineStr">
@@ -944,6 +1155,11 @@
           <t xml:space="preserve">   Item 1</t>
         </is>
       </c>
+      <c r="B50" s="10" t="n"/>
+      <c r="C50" s="10" t="n"/>
+      <c r="D50" s="10" t="n"/>
+      <c r="E50" s="10" t="n"/>
+      <c r="F50" s="11" t="n"/>
       <c r="G50" s="5" t="n"/>
       <c r="H50" s="5" t="n"/>
       <c r="I50" s="5" t="n"/>
@@ -954,6 +1170,11 @@
           <t xml:space="preserve">   Item 2</t>
         </is>
       </c>
+      <c r="B51" s="10" t="n"/>
+      <c r="C51" s="10" t="n"/>
+      <c r="D51" s="10" t="n"/>
+      <c r="E51" s="10" t="n"/>
+      <c r="F51" s="11" t="n"/>
       <c r="G51" s="5" t="n"/>
       <c r="H51" s="5" t="n"/>
       <c r="I51" s="5" t="n"/>
@@ -964,6 +1185,11 @@
           <t xml:space="preserve">   Item 3</t>
         </is>
       </c>
+      <c r="B52" s="10" t="n"/>
+      <c r="C52" s="10" t="n"/>
+      <c r="D52" s="10" t="n"/>
+      <c r="E52" s="10" t="n"/>
+      <c r="F52" s="11" t="n"/>
       <c r="G52" s="5" t="n"/>
       <c r="H52" s="5" t="n"/>
       <c r="I52" s="5" t="n"/>
@@ -974,6 +1200,11 @@
           <t xml:space="preserve">   Item 4</t>
         </is>
       </c>
+      <c r="B53" s="10" t="n"/>
+      <c r="C53" s="10" t="n"/>
+      <c r="D53" s="10" t="n"/>
+      <c r="E53" s="10" t="n"/>
+      <c r="F53" s="11" t="n"/>
       <c r="G53" s="5" t="n"/>
       <c r="H53" s="5" t="n"/>
       <c r="I53" s="5" t="n"/>
@@ -984,6 +1215,11 @@
           <t xml:space="preserve">   Item 5</t>
         </is>
       </c>
+      <c r="B54" s="10" t="n"/>
+      <c r="C54" s="10" t="n"/>
+      <c r="D54" s="10" t="n"/>
+      <c r="E54" s="10" t="n"/>
+      <c r="F54" s="11" t="n"/>
       <c r="G54" s="5" t="n"/>
       <c r="H54" s="5" t="n"/>
       <c r="I54" s="5" t="n"/>
@@ -994,6 +1230,11 @@
           <t xml:space="preserve">   Item 6</t>
         </is>
       </c>
+      <c r="B55" s="10" t="n"/>
+      <c r="C55" s="10" t="n"/>
+      <c r="D55" s="10" t="n"/>
+      <c r="E55" s="10" t="n"/>
+      <c r="F55" s="11" t="n"/>
       <c r="G55" s="5" t="n"/>
       <c r="H55" s="5" t="n"/>
       <c r="I55" s="5" t="n"/>
@@ -1004,6 +1245,11 @@
           <t xml:space="preserve">   Item 7</t>
         </is>
       </c>
+      <c r="B56" s="10" t="n"/>
+      <c r="C56" s="10" t="n"/>
+      <c r="D56" s="10" t="n"/>
+      <c r="E56" s="10" t="n"/>
+      <c r="F56" s="11" t="n"/>
       <c r="G56" s="5" t="n"/>
       <c r="H56" s="5" t="n"/>
       <c r="I56" s="5" t="n"/>
@@ -1014,6 +1260,11 @@
           <t xml:space="preserve">   Item 8</t>
         </is>
       </c>
+      <c r="B57" s="10" t="n"/>
+      <c r="C57" s="10" t="n"/>
+      <c r="D57" s="10" t="n"/>
+      <c r="E57" s="10" t="n"/>
+      <c r="F57" s="11" t="n"/>
       <c r="G57" s="5" t="n"/>
       <c r="H57" s="5" t="n"/>
       <c r="I57" s="5" t="n"/>
@@ -1024,6 +1275,14 @@
           <t>DEMANDAS EMOCIONALES</t>
         </is>
       </c>
+      <c r="B58" s="10" t="n"/>
+      <c r="C58" s="10" t="n"/>
+      <c r="D58" s="10" t="n"/>
+      <c r="E58" s="10" t="n"/>
+      <c r="F58" s="10" t="n"/>
+      <c r="G58" s="10" t="n"/>
+      <c r="H58" s="10" t="n"/>
+      <c r="I58" s="11" t="n"/>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" s="6" t="inlineStr">
@@ -1031,6 +1290,11 @@
           <t xml:space="preserve">   Item 1</t>
         </is>
       </c>
+      <c r="B59" s="10" t="n"/>
+      <c r="C59" s="10" t="n"/>
+      <c r="D59" s="10" t="n"/>
+      <c r="E59" s="10" t="n"/>
+      <c r="F59" s="11" t="n"/>
       <c r="G59" s="5" t="n"/>
       <c r="H59" s="5" t="n"/>
       <c r="I59" s="5" t="n"/>
@@ -1041,6 +1305,11 @@
           <t xml:space="preserve">   Item 2</t>
         </is>
       </c>
+      <c r="B60" s="10" t="n"/>
+      <c r="C60" s="10" t="n"/>
+      <c r="D60" s="10" t="n"/>
+      <c r="E60" s="10" t="n"/>
+      <c r="F60" s="11" t="n"/>
       <c r="G60" s="5" t="n"/>
       <c r="H60" s="5" t="n"/>
       <c r="I60" s="5" t="n"/>
@@ -1051,6 +1320,11 @@
           <t xml:space="preserve">   Item 3</t>
         </is>
       </c>
+      <c r="B61" s="10" t="n"/>
+      <c r="C61" s="10" t="n"/>
+      <c r="D61" s="10" t="n"/>
+      <c r="E61" s="10" t="n"/>
+      <c r="F61" s="11" t="n"/>
       <c r="G61" s="5" t="n"/>
       <c r="H61" s="5" t="n"/>
       <c r="I61" s="5" t="n"/>
@@ -1061,6 +1335,11 @@
           <t xml:space="preserve">   Item 4</t>
         </is>
       </c>
+      <c r="B62" s="10" t="n"/>
+      <c r="C62" s="10" t="n"/>
+      <c r="D62" s="10" t="n"/>
+      <c r="E62" s="10" t="n"/>
+      <c r="F62" s="11" t="n"/>
       <c r="G62" s="5" t="n"/>
       <c r="H62" s="5" t="n"/>
       <c r="I62" s="5" t="n"/>
@@ -1071,6 +1350,11 @@
           <t xml:space="preserve">   Item 5</t>
         </is>
       </c>
+      <c r="B63" s="10" t="n"/>
+      <c r="C63" s="10" t="n"/>
+      <c r="D63" s="10" t="n"/>
+      <c r="E63" s="10" t="n"/>
+      <c r="F63" s="11" t="n"/>
       <c r="G63" s="5" t="n"/>
       <c r="H63" s="5" t="n"/>
       <c r="I63" s="5" t="n"/>
@@ -1081,6 +1365,11 @@
           <t xml:space="preserve">   Item 6</t>
         </is>
       </c>
+      <c r="B64" s="10" t="n"/>
+      <c r="C64" s="10" t="n"/>
+      <c r="D64" s="10" t="n"/>
+      <c r="E64" s="10" t="n"/>
+      <c r="F64" s="11" t="n"/>
       <c r="G64" s="5" t="n"/>
       <c r="H64" s="5" t="n"/>
       <c r="I64" s="5" t="n"/>
@@ -1091,6 +1380,14 @@
           <t>EXIGENCIAS DE RESPONSABILIDAD</t>
         </is>
       </c>
+      <c r="B65" s="10" t="n"/>
+      <c r="C65" s="10" t="n"/>
+      <c r="D65" s="10" t="n"/>
+      <c r="E65" s="10" t="n"/>
+      <c r="F65" s="10" t="n"/>
+      <c r="G65" s="10" t="n"/>
+      <c r="H65" s="10" t="n"/>
+      <c r="I65" s="11" t="n"/>
     </row>
     <row r="66" ht="20" customHeight="1">
       <c r="A66" s="6" t="inlineStr">
@@ -1098,6 +1395,11 @@
           <t xml:space="preserve">   Item 1</t>
         </is>
       </c>
+      <c r="B66" s="10" t="n"/>
+      <c r="C66" s="10" t="n"/>
+      <c r="D66" s="10" t="n"/>
+      <c r="E66" s="10" t="n"/>
+      <c r="F66" s="11" t="n"/>
       <c r="G66" s="5" t="n"/>
       <c r="H66" s="5" t="n"/>
       <c r="I66" s="5" t="n"/>
@@ -1108,6 +1410,11 @@
           <t xml:space="preserve">   Item 2</t>
         </is>
       </c>
+      <c r="B67" s="10" t="n"/>
+      <c r="C67" s="10" t="n"/>
+      <c r="D67" s="10" t="n"/>
+      <c r="E67" s="10" t="n"/>
+      <c r="F67" s="11" t="n"/>
       <c r="G67" s="5" t="n"/>
       <c r="H67" s="5" t="n"/>
       <c r="I67" s="5" t="n"/>
@@ -1118,6 +1425,11 @@
           <t xml:space="preserve">   Item 3</t>
         </is>
       </c>
+      <c r="B68" s="10" t="n"/>
+      <c r="C68" s="10" t="n"/>
+      <c r="D68" s="10" t="n"/>
+      <c r="E68" s="10" t="n"/>
+      <c r="F68" s="11" t="n"/>
       <c r="G68" s="5" t="n"/>
       <c r="H68" s="5" t="n"/>
       <c r="I68" s="5" t="n"/>
@@ -1128,6 +1440,11 @@
           <t xml:space="preserve">   Item 4</t>
         </is>
       </c>
+      <c r="B69" s="10" t="n"/>
+      <c r="C69" s="10" t="n"/>
+      <c r="D69" s="10" t="n"/>
+      <c r="E69" s="10" t="n"/>
+      <c r="F69" s="11" t="n"/>
       <c r="G69" s="5" t="n"/>
       <c r="H69" s="5" t="n"/>
       <c r="I69" s="5" t="n"/>
@@ -1138,6 +1455,11 @@
           <t xml:space="preserve">   Item 5</t>
         </is>
       </c>
+      <c r="B70" s="10" t="n"/>
+      <c r="C70" s="10" t="n"/>
+      <c r="D70" s="10" t="n"/>
+      <c r="E70" s="10" t="n"/>
+      <c r="F70" s="11" t="n"/>
       <c r="G70" s="5" t="n"/>
       <c r="H70" s="5" t="n"/>
       <c r="I70" s="5" t="n"/>
@@ -1148,6 +1470,11 @@
           <t xml:space="preserve">   Item 6</t>
         </is>
       </c>
+      <c r="B71" s="10" t="n"/>
+      <c r="C71" s="10" t="n"/>
+      <c r="D71" s="10" t="n"/>
+      <c r="E71" s="10" t="n"/>
+      <c r="F71" s="11" t="n"/>
       <c r="G71" s="5" t="n"/>
       <c r="H71" s="5" t="n"/>
       <c r="I71" s="5" t="n"/>
@@ -1158,6 +1485,14 @@
           <t>CONSISTENCIA DE ROL</t>
         </is>
       </c>
+      <c r="B72" s="10" t="n"/>
+      <c r="C72" s="10" t="n"/>
+      <c r="D72" s="10" t="n"/>
+      <c r="E72" s="10" t="n"/>
+      <c r="F72" s="10" t="n"/>
+      <c r="G72" s="10" t="n"/>
+      <c r="H72" s="10" t="n"/>
+      <c r="I72" s="11" t="n"/>
     </row>
     <row r="73" ht="20" customHeight="1">
       <c r="A73" s="6" t="inlineStr">
@@ -1165,6 +1500,11 @@
           <t xml:space="preserve">   Item 1</t>
         </is>
       </c>
+      <c r="B73" s="10" t="n"/>
+      <c r="C73" s="10" t="n"/>
+      <c r="D73" s="10" t="n"/>
+      <c r="E73" s="10" t="n"/>
+      <c r="F73" s="11" t="n"/>
       <c r="G73" s="5" t="n"/>
       <c r="H73" s="5" t="n"/>
       <c r="I73" s="5" t="n"/>
@@ -1175,6 +1515,11 @@
           <t xml:space="preserve">   Item 2</t>
         </is>
       </c>
+      <c r="B74" s="10" t="n"/>
+      <c r="C74" s="10" t="n"/>
+      <c r="D74" s="10" t="n"/>
+      <c r="E74" s="10" t="n"/>
+      <c r="F74" s="11" t="n"/>
       <c r="G74" s="5" t="n"/>
       <c r="H74" s="5" t="n"/>
       <c r="I74" s="5" t="n"/>
@@ -1185,6 +1530,11 @@
           <t xml:space="preserve">   Item 3</t>
         </is>
       </c>
+      <c r="B75" s="10" t="n"/>
+      <c r="C75" s="10" t="n"/>
+      <c r="D75" s="10" t="n"/>
+      <c r="E75" s="10" t="n"/>
+      <c r="F75" s="11" t="n"/>
       <c r="G75" s="5" t="n"/>
       <c r="H75" s="5" t="n"/>
       <c r="I75" s="5" t="n"/>
@@ -1195,6 +1545,11 @@
           <t xml:space="preserve">   Item 4</t>
         </is>
       </c>
+      <c r="B76" s="10" t="n"/>
+      <c r="C76" s="10" t="n"/>
+      <c r="D76" s="10" t="n"/>
+      <c r="E76" s="10" t="n"/>
+      <c r="F76" s="11" t="n"/>
       <c r="G76" s="5" t="n"/>
       <c r="H76" s="5" t="n"/>
       <c r="I76" s="5" t="n"/>
@@ -1205,6 +1560,11 @@
           <t xml:space="preserve">   Item 5</t>
         </is>
       </c>
+      <c r="B77" s="10" t="n"/>
+      <c r="C77" s="10" t="n"/>
+      <c r="D77" s="10" t="n"/>
+      <c r="E77" s="10" t="n"/>
+      <c r="F77" s="11" t="n"/>
       <c r="G77" s="5" t="n"/>
       <c r="H77" s="5" t="n"/>
       <c r="I77" s="5" t="n"/>
@@ -1215,6 +1575,11 @@
           <t xml:space="preserve">   Item 6</t>
         </is>
       </c>
+      <c r="B78" s="10" t="n"/>
+      <c r="C78" s="10" t="n"/>
+      <c r="D78" s="10" t="n"/>
+      <c r="E78" s="10" t="n"/>
+      <c r="F78" s="11" t="n"/>
       <c r="G78" s="5" t="n"/>
       <c r="H78" s="5" t="n"/>
       <c r="I78" s="5" t="n"/>
@@ -1225,6 +1590,11 @@
           <t xml:space="preserve">   Item 7</t>
         </is>
       </c>
+      <c r="B79" s="10" t="n"/>
+      <c r="C79" s="10" t="n"/>
+      <c r="D79" s="10" t="n"/>
+      <c r="E79" s="10" t="n"/>
+      <c r="F79" s="11" t="n"/>
       <c r="G79" s="5" t="n"/>
       <c r="H79" s="5" t="n"/>
       <c r="I79" s="5" t="n"/>
@@ -1235,6 +1605,14 @@
           <t>DEMANDAS AMBIENTALES Y ESFUERZO FÍSICO</t>
         </is>
       </c>
+      <c r="B80" s="10" t="n"/>
+      <c r="C80" s="10" t="n"/>
+      <c r="D80" s="10" t="n"/>
+      <c r="E80" s="10" t="n"/>
+      <c r="F80" s="10" t="n"/>
+      <c r="G80" s="10" t="n"/>
+      <c r="H80" s="10" t="n"/>
+      <c r="I80" s="11" t="n"/>
     </row>
     <row r="81" ht="20" customHeight="1">
       <c r="A81" s="6" t="inlineStr">
@@ -1242,6 +1620,11 @@
           <t xml:space="preserve">   Item 1</t>
         </is>
       </c>
+      <c r="B81" s="10" t="n"/>
+      <c r="C81" s="10" t="n"/>
+      <c r="D81" s="10" t="n"/>
+      <c r="E81" s="10" t="n"/>
+      <c r="F81" s="11" t="n"/>
       <c r="G81" s="5" t="n"/>
       <c r="H81" s="5" t="n"/>
       <c r="I81" s="5" t="n"/>
@@ -1252,6 +1635,11 @@
           <t xml:space="preserve">   Item 2</t>
         </is>
       </c>
+      <c r="B82" s="10" t="n"/>
+      <c r="C82" s="10" t="n"/>
+      <c r="D82" s="10" t="n"/>
+      <c r="E82" s="10" t="n"/>
+      <c r="F82" s="11" t="n"/>
       <c r="G82" s="5" t="n"/>
       <c r="H82" s="5" t="n"/>
       <c r="I82" s="5" t="n"/>
@@ -1262,6 +1650,11 @@
           <t xml:space="preserve">   Item 3</t>
         </is>
       </c>
+      <c r="B83" s="10" t="n"/>
+      <c r="C83" s="10" t="n"/>
+      <c r="D83" s="10" t="n"/>
+      <c r="E83" s="10" t="n"/>
+      <c r="F83" s="11" t="n"/>
       <c r="G83" s="5" t="n"/>
       <c r="H83" s="5" t="n"/>
       <c r="I83" s="5" t="n"/>
@@ -1272,6 +1665,11 @@
           <t xml:space="preserve">   Item 4</t>
         </is>
       </c>
+      <c r="B84" s="10" t="n"/>
+      <c r="C84" s="10" t="n"/>
+      <c r="D84" s="10" t="n"/>
+      <c r="E84" s="10" t="n"/>
+      <c r="F84" s="11" t="n"/>
       <c r="G84" s="5" t="n"/>
       <c r="H84" s="5" t="n"/>
       <c r="I84" s="5" t="n"/>
@@ -1282,6 +1680,11 @@
           <t xml:space="preserve">   Item 5</t>
         </is>
       </c>
+      <c r="B85" s="10" t="n"/>
+      <c r="C85" s="10" t="n"/>
+      <c r="D85" s="10" t="n"/>
+      <c r="E85" s="10" t="n"/>
+      <c r="F85" s="11" t="n"/>
       <c r="G85" s="5" t="n"/>
       <c r="H85" s="5" t="n"/>
       <c r="I85" s="5" t="n"/>
@@ -1292,6 +1695,11 @@
           <t xml:space="preserve">   Item 6</t>
         </is>
       </c>
+      <c r="B86" s="10" t="n"/>
+      <c r="C86" s="10" t="n"/>
+      <c r="D86" s="10" t="n"/>
+      <c r="E86" s="10" t="n"/>
+      <c r="F86" s="11" t="n"/>
       <c r="G86" s="5" t="n"/>
       <c r="H86" s="5" t="n"/>
       <c r="I86" s="5" t="n"/>
@@ -1302,6 +1710,11 @@
           <t xml:space="preserve">   Item 7</t>
         </is>
       </c>
+      <c r="B87" s="10" t="n"/>
+      <c r="C87" s="10" t="n"/>
+      <c r="D87" s="10" t="n"/>
+      <c r="E87" s="10" t="n"/>
+      <c r="F87" s="11" t="n"/>
       <c r="G87" s="5" t="n"/>
       <c r="H87" s="5" t="n"/>
       <c r="I87" s="5" t="n"/>
@@ -1312,6 +1725,11 @@
           <t xml:space="preserve">   Item 8</t>
         </is>
       </c>
+      <c r="B88" s="10" t="n"/>
+      <c r="C88" s="10" t="n"/>
+      <c r="D88" s="10" t="n"/>
+      <c r="E88" s="10" t="n"/>
+      <c r="F88" s="11" t="n"/>
       <c r="G88" s="5" t="n"/>
       <c r="H88" s="5" t="n"/>
       <c r="I88" s="5" t="n"/>
@@ -1322,6 +1740,11 @@
           <t xml:space="preserve">   Item 9</t>
         </is>
       </c>
+      <c r="B89" s="10" t="n"/>
+      <c r="C89" s="10" t="n"/>
+      <c r="D89" s="10" t="n"/>
+      <c r="E89" s="10" t="n"/>
+      <c r="F89" s="11" t="n"/>
       <c r="G89" s="5" t="n"/>
       <c r="H89" s="5" t="n"/>
       <c r="I89" s="5" t="n"/>
@@ -1332,6 +1755,11 @@
           <t xml:space="preserve">   Item 10</t>
         </is>
       </c>
+      <c r="B90" s="10" t="n"/>
+      <c r="C90" s="10" t="n"/>
+      <c r="D90" s="10" t="n"/>
+      <c r="E90" s="10" t="n"/>
+      <c r="F90" s="11" t="n"/>
       <c r="G90" s="5" t="n"/>
       <c r="H90" s="5" t="n"/>
       <c r="I90" s="5" t="n"/>
@@ -1342,6 +1770,11 @@
           <t xml:space="preserve">   Item 11</t>
         </is>
       </c>
+      <c r="B91" s="10" t="n"/>
+      <c r="C91" s="10" t="n"/>
+      <c r="D91" s="10" t="n"/>
+      <c r="E91" s="10" t="n"/>
+      <c r="F91" s="11" t="n"/>
       <c r="G91" s="5" t="n"/>
       <c r="H91" s="5" t="n"/>
       <c r="I91" s="5" t="n"/>
@@ -1352,6 +1785,11 @@
           <t xml:space="preserve">   Item 12</t>
         </is>
       </c>
+      <c r="B92" s="10" t="n"/>
+      <c r="C92" s="10" t="n"/>
+      <c r="D92" s="10" t="n"/>
+      <c r="E92" s="10" t="n"/>
+      <c r="F92" s="11" t="n"/>
       <c r="G92" s="5" t="n"/>
       <c r="H92" s="5" t="n"/>
       <c r="I92" s="5" t="n"/>
@@ -1362,6 +1800,11 @@
           <t xml:space="preserve">   Item 13</t>
         </is>
       </c>
+      <c r="B93" s="10" t="n"/>
+      <c r="C93" s="10" t="n"/>
+      <c r="D93" s="10" t="n"/>
+      <c r="E93" s="10" t="n"/>
+      <c r="F93" s="11" t="n"/>
       <c r="G93" s="5" t="n"/>
       <c r="H93" s="5" t="n"/>
       <c r="I93" s="5" t="n"/>
@@ -1372,6 +1815,11 @@
           <t xml:space="preserve">   Item 14</t>
         </is>
       </c>
+      <c r="B94" s="10" t="n"/>
+      <c r="C94" s="10" t="n"/>
+      <c r="D94" s="10" t="n"/>
+      <c r="E94" s="10" t="n"/>
+      <c r="F94" s="11" t="n"/>
       <c r="G94" s="5" t="n"/>
       <c r="H94" s="5" t="n"/>
       <c r="I94" s="5" t="n"/>
@@ -1382,6 +1830,14 @@
           <t>DEMANDAS DE JORNADA</t>
         </is>
       </c>
+      <c r="B95" s="10" t="n"/>
+      <c r="C95" s="10" t="n"/>
+      <c r="D95" s="10" t="n"/>
+      <c r="E95" s="10" t="n"/>
+      <c r="F95" s="10" t="n"/>
+      <c r="G95" s="10" t="n"/>
+      <c r="H95" s="10" t="n"/>
+      <c r="I95" s="11" t="n"/>
     </row>
     <row r="96" ht="20" customHeight="1">
       <c r="A96" s="6" t="inlineStr">
@@ -1389,6 +1845,11 @@
           <t xml:space="preserve">   Item 1</t>
         </is>
       </c>
+      <c r="B96" s="10" t="n"/>
+      <c r="C96" s="10" t="n"/>
+      <c r="D96" s="10" t="n"/>
+      <c r="E96" s="10" t="n"/>
+      <c r="F96" s="11" t="n"/>
       <c r="G96" s="5" t="n"/>
       <c r="H96" s="5" t="n"/>
       <c r="I96" s="5" t="n"/>
@@ -1399,6 +1860,11 @@
           <t xml:space="preserve">   Item 2</t>
         </is>
       </c>
+      <c r="B97" s="10" t="n"/>
+      <c r="C97" s="10" t="n"/>
+      <c r="D97" s="10" t="n"/>
+      <c r="E97" s="10" t="n"/>
+      <c r="F97" s="11" t="n"/>
       <c r="G97" s="5" t="n"/>
       <c r="H97" s="5" t="n"/>
       <c r="I97" s="5" t="n"/>
@@ -1409,6 +1875,11 @@
           <t xml:space="preserve">   Item 3</t>
         </is>
       </c>
+      <c r="B98" s="10" t="n"/>
+      <c r="C98" s="10" t="n"/>
+      <c r="D98" s="10" t="n"/>
+      <c r="E98" s="10" t="n"/>
+      <c r="F98" s="11" t="n"/>
       <c r="G98" s="5" t="n"/>
       <c r="H98" s="5" t="n"/>
       <c r="I98" s="5" t="n"/>
@@ -1419,6 +1890,11 @@
           <t xml:space="preserve">   Item 4</t>
         </is>
       </c>
+      <c r="B99" s="10" t="n"/>
+      <c r="C99" s="10" t="n"/>
+      <c r="D99" s="10" t="n"/>
+      <c r="E99" s="10" t="n"/>
+      <c r="F99" s="11" t="n"/>
       <c r="G99" s="5" t="n"/>
       <c r="H99" s="5" t="n"/>
       <c r="I99" s="5" t="n"/>
@@ -1437,6 +1913,13 @@
         </is>
       </c>
       <c r="B102" s="6" t="n"/>
+      <c r="C102" s="10" t="n"/>
+      <c r="D102" s="10" t="n"/>
+      <c r="E102" s="10" t="n"/>
+      <c r="F102" s="10" t="n"/>
+      <c r="G102" s="10" t="n"/>
+      <c r="H102" s="10" t="n"/>
+      <c r="I102" s="11" t="n"/>
     </row>
     <row r="103" ht="30" customHeight="1">
       <c r="A103" s="4" t="inlineStr">
@@ -1445,6 +1928,13 @@
         </is>
       </c>
       <c r="B103" s="6" t="n"/>
+      <c r="C103" s="10" t="n"/>
+      <c r="D103" s="10" t="n"/>
+      <c r="E103" s="10" t="n"/>
+      <c r="F103" s="10" t="n"/>
+      <c r="G103" s="10" t="n"/>
+      <c r="H103" s="10" t="n"/>
+      <c r="I103" s="11" t="n"/>
     </row>
     <row r="104" ht="60" customHeight="1">
       <c r="A104" s="4" t="inlineStr">
@@ -1453,6 +1943,13 @@
         </is>
       </c>
       <c r="B104" s="6" t="n"/>
+      <c r="C104" s="10" t="n"/>
+      <c r="D104" s="10" t="n"/>
+      <c r="E104" s="10" t="n"/>
+      <c r="F104" s="10" t="n"/>
+      <c r="G104" s="10" t="n"/>
+      <c r="H104" s="10" t="n"/>
+      <c r="I104" s="11" t="n"/>
     </row>
     <row r="105" ht="60" customHeight="1">
       <c r="A105" s="4" t="inlineStr">
@@ -1461,6 +1958,13 @@
         </is>
       </c>
       <c r="B105" s="6" t="n"/>
+      <c r="C105" s="10" t="n"/>
+      <c r="D105" s="10" t="n"/>
+      <c r="E105" s="10" t="n"/>
+      <c r="F105" s="10" t="n"/>
+      <c r="G105" s="10" t="n"/>
+      <c r="H105" s="10" t="n"/>
+      <c r="I105" s="11" t="n"/>
     </row>
     <row r="107">
       <c r="A107" s="2" t="inlineStr">
@@ -1469,6 +1973,9 @@
         </is>
       </c>
       <c r="B107" s="5" t="n"/>
+      <c r="C107" s="10" t="n"/>
+      <c r="D107" s="10" t="n"/>
+      <c r="E107" s="11" t="n"/>
     </row>
     <row r="108">
       <c r="A108" s="2" t="inlineStr">
@@ -1477,6 +1984,9 @@
         </is>
       </c>
       <c r="B108" s="5" t="n"/>
+      <c r="C108" s="10" t="n"/>
+      <c r="D108" s="10" t="n"/>
+      <c r="E108" s="11" t="n"/>
     </row>
     <row r="109">
       <c r="A109" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Revert "Fix: Eliminada metadata (Company: Positiva) de plantilla Excel"
This reverts commit 15a3967f514be82d2043eb0a3703f67f9b9091d9.
</commit_message>
<xml_diff>
--- a/backend/app/services/plantilla_valoracion_simple.xlsx
+++ b/backend/app/services/plantilla_valoracion_simple.xlsx
@@ -75,7 +75,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -89,39 +89,11 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -140,8 +112,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -539,6 +509,9 @@
           <t>Fecha de valoración:</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
@@ -554,13 +527,6 @@
         </is>
       </c>
       <c r="B5" s="5" t="n"/>
-      <c r="C5" s="10" t="n"/>
-      <c r="D5" s="10" t="n"/>
-      <c r="E5" s="10" t="n"/>
-      <c r="F5" s="10" t="n"/>
-      <c r="G5" s="10" t="n"/>
-      <c r="H5" s="10" t="n"/>
-      <c r="I5" s="11" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
@@ -569,13 +535,6 @@
         </is>
       </c>
       <c r="B6" s="5" t="n"/>
-      <c r="C6" s="10" t="n"/>
-      <c r="D6" s="10" t="n"/>
-      <c r="E6" s="10" t="n"/>
-      <c r="F6" s="10" t="n"/>
-      <c r="G6" s="10" t="n"/>
-      <c r="H6" s="10" t="n"/>
-      <c r="I6" s="11" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
@@ -583,6 +542,9 @@
           <t>Fecha de nacimiento:</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
       <c r="F7" s="2" t="inlineStr">
         <is>
           <t>Edad:</t>
@@ -646,13 +608,6 @@
         </is>
       </c>
       <c r="B10" s="6" t="n"/>
-      <c r="C10" s="10" t="n"/>
-      <c r="D10" s="10" t="n"/>
-      <c r="E10" s="10" t="n"/>
-      <c r="F10" s="10" t="n"/>
-      <c r="G10" s="10" t="n"/>
-      <c r="H10" s="10" t="n"/>
-      <c r="I10" s="11" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
@@ -661,13 +616,6 @@
         </is>
       </c>
       <c r="B11" s="5" t="n"/>
-      <c r="C11" s="10" t="n"/>
-      <c r="D11" s="10" t="n"/>
-      <c r="E11" s="10" t="n"/>
-      <c r="F11" s="10" t="n"/>
-      <c r="G11" s="10" t="n"/>
-      <c r="H11" s="10" t="n"/>
-      <c r="I11" s="11" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="4" t="inlineStr">
@@ -676,13 +624,6 @@
         </is>
       </c>
       <c r="B12" s="5" t="n"/>
-      <c r="C12" s="10" t="n"/>
-      <c r="D12" s="10" t="n"/>
-      <c r="E12" s="10" t="n"/>
-      <c r="F12" s="10" t="n"/>
-      <c r="G12" s="10" t="n"/>
-      <c r="H12" s="10" t="n"/>
-      <c r="I12" s="11" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
@@ -691,13 +632,6 @@
         </is>
       </c>
       <c r="B13" s="5" t="n"/>
-      <c r="C13" s="10" t="n"/>
-      <c r="D13" s="10" t="n"/>
-      <c r="E13" s="10" t="n"/>
-      <c r="F13" s="10" t="n"/>
-      <c r="G13" s="10" t="n"/>
-      <c r="H13" s="10" t="n"/>
-      <c r="I13" s="11" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="4" t="inlineStr">
@@ -750,13 +684,6 @@
         </is>
       </c>
       <c r="B18" s="5" t="n"/>
-      <c r="C18" s="10" t="n"/>
-      <c r="D18" s="10" t="n"/>
-      <c r="E18" s="10" t="n"/>
-      <c r="F18" s="10" t="n"/>
-      <c r="G18" s="10" t="n"/>
-      <c r="H18" s="10" t="n"/>
-      <c r="I18" s="11" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
@@ -765,13 +692,6 @@
         </is>
       </c>
       <c r="B19" s="5" t="n"/>
-      <c r="C19" s="10" t="n"/>
-      <c r="D19" s="10" t="n"/>
-      <c r="E19" s="10" t="n"/>
-      <c r="F19" s="10" t="n"/>
-      <c r="G19" s="10" t="n"/>
-      <c r="H19" s="10" t="n"/>
-      <c r="I19" s="11" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
@@ -794,13 +714,6 @@
         </is>
       </c>
       <c r="B21" s="5" t="n"/>
-      <c r="C21" s="10" t="n"/>
-      <c r="D21" s="10" t="n"/>
-      <c r="E21" s="10" t="n"/>
-      <c r="F21" s="10" t="n"/>
-      <c r="G21" s="10" t="n"/>
-      <c r="H21" s="10" t="n"/>
-      <c r="I21" s="11" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
@@ -809,13 +722,6 @@
         </is>
       </c>
       <c r="B22" s="5" t="n"/>
-      <c r="C22" s="10" t="n"/>
-      <c r="D22" s="10" t="n"/>
-      <c r="E22" s="10" t="n"/>
-      <c r="F22" s="10" t="n"/>
-      <c r="G22" s="10" t="n"/>
-      <c r="H22" s="10" t="n"/>
-      <c r="I22" s="11" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="4" t="inlineStr">
@@ -838,13 +744,6 @@
         </is>
       </c>
       <c r="B24" s="5" t="n"/>
-      <c r="C24" s="10" t="n"/>
-      <c r="D24" s="10" t="n"/>
-      <c r="E24" s="10" t="n"/>
-      <c r="F24" s="10" t="n"/>
-      <c r="G24" s="10" t="n"/>
-      <c r="H24" s="10" t="n"/>
-      <c r="I24" s="11" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
@@ -864,54 +763,34 @@
           <t>Cargo/Funciones</t>
         </is>
       </c>
-      <c r="C27" s="10" t="n"/>
-      <c r="D27" s="11" t="n"/>
       <c r="E27" s="7" t="inlineStr">
         <is>
           <t>Duración</t>
         </is>
       </c>
-      <c r="F27" s="11" t="n"/>
       <c r="G27" s="7" t="inlineStr">
         <is>
           <t>Motivo de retiro</t>
         </is>
       </c>
-      <c r="H27" s="10" t="n"/>
-      <c r="I27" s="11" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="n"/>
       <c r="B28" s="5" t="n"/>
-      <c r="C28" s="10" t="n"/>
-      <c r="D28" s="11" t="n"/>
       <c r="E28" s="5" t="n"/>
-      <c r="F28" s="11" t="n"/>
       <c r="G28" s="5" t="n"/>
-      <c r="H28" s="10" t="n"/>
-      <c r="I28" s="11" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="n"/>
       <c r="B29" s="5" t="n"/>
-      <c r="C29" s="10" t="n"/>
-      <c r="D29" s="11" t="n"/>
       <c r="E29" s="5" t="n"/>
-      <c r="F29" s="11" t="n"/>
       <c r="G29" s="5" t="n"/>
-      <c r="H29" s="10" t="n"/>
-      <c r="I29" s="11" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="n"/>
       <c r="B30" s="5" t="n"/>
-      <c r="C30" s="10" t="n"/>
-      <c r="D30" s="11" t="n"/>
       <c r="E30" s="5" t="n"/>
-      <c r="F30" s="11" t="n"/>
       <c r="G30" s="5" t="n"/>
-      <c r="H30" s="10" t="n"/>
-      <c r="I30" s="11" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="4" t="inlineStr">
@@ -920,13 +799,6 @@
         </is>
       </c>
       <c r="B32" s="6" t="n"/>
-      <c r="C32" s="10" t="n"/>
-      <c r="D32" s="10" t="n"/>
-      <c r="E32" s="10" t="n"/>
-      <c r="F32" s="10" t="n"/>
-      <c r="G32" s="10" t="n"/>
-      <c r="H32" s="10" t="n"/>
-      <c r="I32" s="11" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="4" t="inlineStr">
@@ -935,13 +807,6 @@
         </is>
       </c>
       <c r="B33" s="6" t="n"/>
-      <c r="C33" s="10" t="n"/>
-      <c r="D33" s="10" t="n"/>
-      <c r="E33" s="10" t="n"/>
-      <c r="F33" s="10" t="n"/>
-      <c r="G33" s="10" t="n"/>
-      <c r="H33" s="10" t="n"/>
-      <c r="I33" s="11" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
@@ -957,13 +822,6 @@
         </is>
       </c>
       <c r="B36" s="5" t="n"/>
-      <c r="C36" s="10" t="n"/>
-      <c r="D36" s="10" t="n"/>
-      <c r="E36" s="10" t="n"/>
-      <c r="F36" s="10" t="n"/>
-      <c r="G36" s="10" t="n"/>
-      <c r="H36" s="10" t="n"/>
-      <c r="I36" s="11" t="n"/>
     </row>
     <row r="37" ht="30" customHeight="1">
       <c r="A37" s="4" t="inlineStr">
@@ -972,13 +830,6 @@
         </is>
       </c>
       <c r="B37" s="6" t="n"/>
-      <c r="C37" s="10" t="n"/>
-      <c r="D37" s="10" t="n"/>
-      <c r="E37" s="10" t="n"/>
-      <c r="F37" s="10" t="n"/>
-      <c r="G37" s="10" t="n"/>
-      <c r="H37" s="10" t="n"/>
-      <c r="I37" s="11" t="n"/>
     </row>
     <row r="38">
       <c r="A38" s="4" t="inlineStr">
@@ -987,13 +838,6 @@
         </is>
       </c>
       <c r="B38" s="6" t="n"/>
-      <c r="C38" s="10" t="n"/>
-      <c r="D38" s="10" t="n"/>
-      <c r="E38" s="10" t="n"/>
-      <c r="F38" s="10" t="n"/>
-      <c r="G38" s="10" t="n"/>
-      <c r="H38" s="10" t="n"/>
-      <c r="I38" s="11" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="4" t="inlineStr">
@@ -1002,13 +846,6 @@
         </is>
       </c>
       <c r="B39" s="5" t="n"/>
-      <c r="C39" s="10" t="n"/>
-      <c r="D39" s="10" t="n"/>
-      <c r="E39" s="10" t="n"/>
-      <c r="F39" s="10" t="n"/>
-      <c r="G39" s="10" t="n"/>
-      <c r="H39" s="10" t="n"/>
-      <c r="I39" s="11" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="4" t="inlineStr">
@@ -1017,13 +854,6 @@
         </is>
       </c>
       <c r="B40" s="6" t="n"/>
-      <c r="C40" s="10" t="n"/>
-      <c r="D40" s="10" t="n"/>
-      <c r="E40" s="10" t="n"/>
-      <c r="F40" s="10" t="n"/>
-      <c r="G40" s="10" t="n"/>
-      <c r="H40" s="10" t="n"/>
-      <c r="I40" s="11" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
@@ -1038,11 +868,6 @@
           <t>Factor de Riesgo</t>
         </is>
       </c>
-      <c r="B43" s="10" t="n"/>
-      <c r="C43" s="10" t="n"/>
-      <c r="D43" s="10" t="n"/>
-      <c r="E43" s="10" t="n"/>
-      <c r="F43" s="11" t="n"/>
       <c r="G43" s="8" t="inlineStr">
         <is>
           <t>SI</t>
@@ -1065,14 +890,6 @@
           <t>DEMANDAS CUANTITATIVAS</t>
         </is>
       </c>
-      <c r="B44" s="10" t="n"/>
-      <c r="C44" s="10" t="n"/>
-      <c r="D44" s="10" t="n"/>
-      <c r="E44" s="10" t="n"/>
-      <c r="F44" s="10" t="n"/>
-      <c r="G44" s="10" t="n"/>
-      <c r="H44" s="10" t="n"/>
-      <c r="I44" s="11" t="n"/>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="6" t="inlineStr">
@@ -1080,11 +897,6 @@
           <t xml:space="preserve">   Item 1</t>
         </is>
       </c>
-      <c r="B45" s="10" t="n"/>
-      <c r="C45" s="10" t="n"/>
-      <c r="D45" s="10" t="n"/>
-      <c r="E45" s="10" t="n"/>
-      <c r="F45" s="11" t="n"/>
       <c r="G45" s="5" t="n"/>
       <c r="H45" s="5" t="n"/>
       <c r="I45" s="5" t="n"/>
@@ -1095,11 +907,6 @@
           <t xml:space="preserve">   Item 2</t>
         </is>
       </c>
-      <c r="B46" s="10" t="n"/>
-      <c r="C46" s="10" t="n"/>
-      <c r="D46" s="10" t="n"/>
-      <c r="E46" s="10" t="n"/>
-      <c r="F46" s="11" t="n"/>
       <c r="G46" s="5" t="n"/>
       <c r="H46" s="5" t="n"/>
       <c r="I46" s="5" t="n"/>
@@ -1110,11 +917,6 @@
           <t xml:space="preserve">   Item 3</t>
         </is>
       </c>
-      <c r="B47" s="10" t="n"/>
-      <c r="C47" s="10" t="n"/>
-      <c r="D47" s="10" t="n"/>
-      <c r="E47" s="10" t="n"/>
-      <c r="F47" s="11" t="n"/>
       <c r="G47" s="5" t="n"/>
       <c r="H47" s="5" t="n"/>
       <c r="I47" s="5" t="n"/>
@@ -1125,11 +927,6 @@
           <t xml:space="preserve">   Item 4</t>
         </is>
       </c>
-      <c r="B48" s="10" t="n"/>
-      <c r="C48" s="10" t="n"/>
-      <c r="D48" s="10" t="n"/>
-      <c r="E48" s="10" t="n"/>
-      <c r="F48" s="11" t="n"/>
       <c r="G48" s="5" t="n"/>
       <c r="H48" s="5" t="n"/>
       <c r="I48" s="5" t="n"/>
@@ -1140,14 +937,6 @@
           <t>DEMANDAS DE CARGA MENTAL</t>
         </is>
       </c>
-      <c r="B49" s="10" t="n"/>
-      <c r="C49" s="10" t="n"/>
-      <c r="D49" s="10" t="n"/>
-      <c r="E49" s="10" t="n"/>
-      <c r="F49" s="10" t="n"/>
-      <c r="G49" s="10" t="n"/>
-      <c r="H49" s="10" t="n"/>
-      <c r="I49" s="11" t="n"/>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="6" t="inlineStr">
@@ -1155,11 +944,6 @@
           <t xml:space="preserve">   Item 1</t>
         </is>
       </c>
-      <c r="B50" s="10" t="n"/>
-      <c r="C50" s="10" t="n"/>
-      <c r="D50" s="10" t="n"/>
-      <c r="E50" s="10" t="n"/>
-      <c r="F50" s="11" t="n"/>
       <c r="G50" s="5" t="n"/>
       <c r="H50" s="5" t="n"/>
       <c r="I50" s="5" t="n"/>
@@ -1170,11 +954,6 @@
           <t xml:space="preserve">   Item 2</t>
         </is>
       </c>
-      <c r="B51" s="10" t="n"/>
-      <c r="C51" s="10" t="n"/>
-      <c r="D51" s="10" t="n"/>
-      <c r="E51" s="10" t="n"/>
-      <c r="F51" s="11" t="n"/>
       <c r="G51" s="5" t="n"/>
       <c r="H51" s="5" t="n"/>
       <c r="I51" s="5" t="n"/>
@@ -1185,11 +964,6 @@
           <t xml:space="preserve">   Item 3</t>
         </is>
       </c>
-      <c r="B52" s="10" t="n"/>
-      <c r="C52" s="10" t="n"/>
-      <c r="D52" s="10" t="n"/>
-      <c r="E52" s="10" t="n"/>
-      <c r="F52" s="11" t="n"/>
       <c r="G52" s="5" t="n"/>
       <c r="H52" s="5" t="n"/>
       <c r="I52" s="5" t="n"/>
@@ -1200,11 +974,6 @@
           <t xml:space="preserve">   Item 4</t>
         </is>
       </c>
-      <c r="B53" s="10" t="n"/>
-      <c r="C53" s="10" t="n"/>
-      <c r="D53" s="10" t="n"/>
-      <c r="E53" s="10" t="n"/>
-      <c r="F53" s="11" t="n"/>
       <c r="G53" s="5" t="n"/>
       <c r="H53" s="5" t="n"/>
       <c r="I53" s="5" t="n"/>
@@ -1215,11 +984,6 @@
           <t xml:space="preserve">   Item 5</t>
         </is>
       </c>
-      <c r="B54" s="10" t="n"/>
-      <c r="C54" s="10" t="n"/>
-      <c r="D54" s="10" t="n"/>
-      <c r="E54" s="10" t="n"/>
-      <c r="F54" s="11" t="n"/>
       <c r="G54" s="5" t="n"/>
       <c r="H54" s="5" t="n"/>
       <c r="I54" s="5" t="n"/>
@@ -1230,11 +994,6 @@
           <t xml:space="preserve">   Item 6</t>
         </is>
       </c>
-      <c r="B55" s="10" t="n"/>
-      <c r="C55" s="10" t="n"/>
-      <c r="D55" s="10" t="n"/>
-      <c r="E55" s="10" t="n"/>
-      <c r="F55" s="11" t="n"/>
       <c r="G55" s="5" t="n"/>
       <c r="H55" s="5" t="n"/>
       <c r="I55" s="5" t="n"/>
@@ -1245,11 +1004,6 @@
           <t xml:space="preserve">   Item 7</t>
         </is>
       </c>
-      <c r="B56" s="10" t="n"/>
-      <c r="C56" s="10" t="n"/>
-      <c r="D56" s="10" t="n"/>
-      <c r="E56" s="10" t="n"/>
-      <c r="F56" s="11" t="n"/>
       <c r="G56" s="5" t="n"/>
       <c r="H56" s="5" t="n"/>
       <c r="I56" s="5" t="n"/>
@@ -1260,11 +1014,6 @@
           <t xml:space="preserve">   Item 8</t>
         </is>
       </c>
-      <c r="B57" s="10" t="n"/>
-      <c r="C57" s="10" t="n"/>
-      <c r="D57" s="10" t="n"/>
-      <c r="E57" s="10" t="n"/>
-      <c r="F57" s="11" t="n"/>
       <c r="G57" s="5" t="n"/>
       <c r="H57" s="5" t="n"/>
       <c r="I57" s="5" t="n"/>
@@ -1275,14 +1024,6 @@
           <t>DEMANDAS EMOCIONALES</t>
         </is>
       </c>
-      <c r="B58" s="10" t="n"/>
-      <c r="C58" s="10" t="n"/>
-      <c r="D58" s="10" t="n"/>
-      <c r="E58" s="10" t="n"/>
-      <c r="F58" s="10" t="n"/>
-      <c r="G58" s="10" t="n"/>
-      <c r="H58" s="10" t="n"/>
-      <c r="I58" s="11" t="n"/>
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" s="6" t="inlineStr">
@@ -1290,11 +1031,6 @@
           <t xml:space="preserve">   Item 1</t>
         </is>
       </c>
-      <c r="B59" s="10" t="n"/>
-      <c r="C59" s="10" t="n"/>
-      <c r="D59" s="10" t="n"/>
-      <c r="E59" s="10" t="n"/>
-      <c r="F59" s="11" t="n"/>
       <c r="G59" s="5" t="n"/>
       <c r="H59" s="5" t="n"/>
       <c r="I59" s="5" t="n"/>
@@ -1305,11 +1041,6 @@
           <t xml:space="preserve">   Item 2</t>
         </is>
       </c>
-      <c r="B60" s="10" t="n"/>
-      <c r="C60" s="10" t="n"/>
-      <c r="D60" s="10" t="n"/>
-      <c r="E60" s="10" t="n"/>
-      <c r="F60" s="11" t="n"/>
       <c r="G60" s="5" t="n"/>
       <c r="H60" s="5" t="n"/>
       <c r="I60" s="5" t="n"/>
@@ -1320,11 +1051,6 @@
           <t xml:space="preserve">   Item 3</t>
         </is>
       </c>
-      <c r="B61" s="10" t="n"/>
-      <c r="C61" s="10" t="n"/>
-      <c r="D61" s="10" t="n"/>
-      <c r="E61" s="10" t="n"/>
-      <c r="F61" s="11" t="n"/>
       <c r="G61" s="5" t="n"/>
       <c r="H61" s="5" t="n"/>
       <c r="I61" s="5" t="n"/>
@@ -1335,11 +1061,6 @@
           <t xml:space="preserve">   Item 4</t>
         </is>
       </c>
-      <c r="B62" s="10" t="n"/>
-      <c r="C62" s="10" t="n"/>
-      <c r="D62" s="10" t="n"/>
-      <c r="E62" s="10" t="n"/>
-      <c r="F62" s="11" t="n"/>
       <c r="G62" s="5" t="n"/>
       <c r="H62" s="5" t="n"/>
       <c r="I62" s="5" t="n"/>
@@ -1350,11 +1071,6 @@
           <t xml:space="preserve">   Item 5</t>
         </is>
       </c>
-      <c r="B63" s="10" t="n"/>
-      <c r="C63" s="10" t="n"/>
-      <c r="D63" s="10" t="n"/>
-      <c r="E63" s="10" t="n"/>
-      <c r="F63" s="11" t="n"/>
       <c r="G63" s="5" t="n"/>
       <c r="H63" s="5" t="n"/>
       <c r="I63" s="5" t="n"/>
@@ -1365,11 +1081,6 @@
           <t xml:space="preserve">   Item 6</t>
         </is>
       </c>
-      <c r="B64" s="10" t="n"/>
-      <c r="C64" s="10" t="n"/>
-      <c r="D64" s="10" t="n"/>
-      <c r="E64" s="10" t="n"/>
-      <c r="F64" s="11" t="n"/>
       <c r="G64" s="5" t="n"/>
       <c r="H64" s="5" t="n"/>
       <c r="I64" s="5" t="n"/>
@@ -1380,14 +1091,6 @@
           <t>EXIGENCIAS DE RESPONSABILIDAD</t>
         </is>
       </c>
-      <c r="B65" s="10" t="n"/>
-      <c r="C65" s="10" t="n"/>
-      <c r="D65" s="10" t="n"/>
-      <c r="E65" s="10" t="n"/>
-      <c r="F65" s="10" t="n"/>
-      <c r="G65" s="10" t="n"/>
-      <c r="H65" s="10" t="n"/>
-      <c r="I65" s="11" t="n"/>
     </row>
     <row r="66" ht="20" customHeight="1">
       <c r="A66" s="6" t="inlineStr">
@@ -1395,11 +1098,6 @@
           <t xml:space="preserve">   Item 1</t>
         </is>
       </c>
-      <c r="B66" s="10" t="n"/>
-      <c r="C66" s="10" t="n"/>
-      <c r="D66" s="10" t="n"/>
-      <c r="E66" s="10" t="n"/>
-      <c r="F66" s="11" t="n"/>
       <c r="G66" s="5" t="n"/>
       <c r="H66" s="5" t="n"/>
       <c r="I66" s="5" t="n"/>
@@ -1410,11 +1108,6 @@
           <t xml:space="preserve">   Item 2</t>
         </is>
       </c>
-      <c r="B67" s="10" t="n"/>
-      <c r="C67" s="10" t="n"/>
-      <c r="D67" s="10" t="n"/>
-      <c r="E67" s="10" t="n"/>
-      <c r="F67" s="11" t="n"/>
       <c r="G67" s="5" t="n"/>
       <c r="H67" s="5" t="n"/>
       <c r="I67" s="5" t="n"/>
@@ -1425,11 +1118,6 @@
           <t xml:space="preserve">   Item 3</t>
         </is>
       </c>
-      <c r="B68" s="10" t="n"/>
-      <c r="C68" s="10" t="n"/>
-      <c r="D68" s="10" t="n"/>
-      <c r="E68" s="10" t="n"/>
-      <c r="F68" s="11" t="n"/>
       <c r="G68" s="5" t="n"/>
       <c r="H68" s="5" t="n"/>
       <c r="I68" s="5" t="n"/>
@@ -1440,11 +1128,6 @@
           <t xml:space="preserve">   Item 4</t>
         </is>
       </c>
-      <c r="B69" s="10" t="n"/>
-      <c r="C69" s="10" t="n"/>
-      <c r="D69" s="10" t="n"/>
-      <c r="E69" s="10" t="n"/>
-      <c r="F69" s="11" t="n"/>
       <c r="G69" s="5" t="n"/>
       <c r="H69" s="5" t="n"/>
       <c r="I69" s="5" t="n"/>
@@ -1455,11 +1138,6 @@
           <t xml:space="preserve">   Item 5</t>
         </is>
       </c>
-      <c r="B70" s="10" t="n"/>
-      <c r="C70" s="10" t="n"/>
-      <c r="D70" s="10" t="n"/>
-      <c r="E70" s="10" t="n"/>
-      <c r="F70" s="11" t="n"/>
       <c r="G70" s="5" t="n"/>
       <c r="H70" s="5" t="n"/>
       <c r="I70" s="5" t="n"/>
@@ -1470,11 +1148,6 @@
           <t xml:space="preserve">   Item 6</t>
         </is>
       </c>
-      <c r="B71" s="10" t="n"/>
-      <c r="C71" s="10" t="n"/>
-      <c r="D71" s="10" t="n"/>
-      <c r="E71" s="10" t="n"/>
-      <c r="F71" s="11" t="n"/>
       <c r="G71" s="5" t="n"/>
       <c r="H71" s="5" t="n"/>
       <c r="I71" s="5" t="n"/>
@@ -1485,14 +1158,6 @@
           <t>CONSISTENCIA DE ROL</t>
         </is>
       </c>
-      <c r="B72" s="10" t="n"/>
-      <c r="C72" s="10" t="n"/>
-      <c r="D72" s="10" t="n"/>
-      <c r="E72" s="10" t="n"/>
-      <c r="F72" s="10" t="n"/>
-      <c r="G72" s="10" t="n"/>
-      <c r="H72" s="10" t="n"/>
-      <c r="I72" s="11" t="n"/>
     </row>
     <row r="73" ht="20" customHeight="1">
       <c r="A73" s="6" t="inlineStr">
@@ -1500,11 +1165,6 @@
           <t xml:space="preserve">   Item 1</t>
         </is>
       </c>
-      <c r="B73" s="10" t="n"/>
-      <c r="C73" s="10" t="n"/>
-      <c r="D73" s="10" t="n"/>
-      <c r="E73" s="10" t="n"/>
-      <c r="F73" s="11" t="n"/>
       <c r="G73" s="5" t="n"/>
       <c r="H73" s="5" t="n"/>
       <c r="I73" s="5" t="n"/>
@@ -1515,11 +1175,6 @@
           <t xml:space="preserve">   Item 2</t>
         </is>
       </c>
-      <c r="B74" s="10" t="n"/>
-      <c r="C74" s="10" t="n"/>
-      <c r="D74" s="10" t="n"/>
-      <c r="E74" s="10" t="n"/>
-      <c r="F74" s="11" t="n"/>
       <c r="G74" s="5" t="n"/>
       <c r="H74" s="5" t="n"/>
       <c r="I74" s="5" t="n"/>
@@ -1530,11 +1185,6 @@
           <t xml:space="preserve">   Item 3</t>
         </is>
       </c>
-      <c r="B75" s="10" t="n"/>
-      <c r="C75" s="10" t="n"/>
-      <c r="D75" s="10" t="n"/>
-      <c r="E75" s="10" t="n"/>
-      <c r="F75" s="11" t="n"/>
       <c r="G75" s="5" t="n"/>
       <c r="H75" s="5" t="n"/>
       <c r="I75" s="5" t="n"/>
@@ -1545,11 +1195,6 @@
           <t xml:space="preserve">   Item 4</t>
         </is>
       </c>
-      <c r="B76" s="10" t="n"/>
-      <c r="C76" s="10" t="n"/>
-      <c r="D76" s="10" t="n"/>
-      <c r="E76" s="10" t="n"/>
-      <c r="F76" s="11" t="n"/>
       <c r="G76" s="5" t="n"/>
       <c r="H76" s="5" t="n"/>
       <c r="I76" s="5" t="n"/>
@@ -1560,11 +1205,6 @@
           <t xml:space="preserve">   Item 5</t>
         </is>
       </c>
-      <c r="B77" s="10" t="n"/>
-      <c r="C77" s="10" t="n"/>
-      <c r="D77" s="10" t="n"/>
-      <c r="E77" s="10" t="n"/>
-      <c r="F77" s="11" t="n"/>
       <c r="G77" s="5" t="n"/>
       <c r="H77" s="5" t="n"/>
       <c r="I77" s="5" t="n"/>
@@ -1575,11 +1215,6 @@
           <t xml:space="preserve">   Item 6</t>
         </is>
       </c>
-      <c r="B78" s="10" t="n"/>
-      <c r="C78" s="10" t="n"/>
-      <c r="D78" s="10" t="n"/>
-      <c r="E78" s="10" t="n"/>
-      <c r="F78" s="11" t="n"/>
       <c r="G78" s="5" t="n"/>
       <c r="H78" s="5" t="n"/>
       <c r="I78" s="5" t="n"/>
@@ -1590,11 +1225,6 @@
           <t xml:space="preserve">   Item 7</t>
         </is>
       </c>
-      <c r="B79" s="10" t="n"/>
-      <c r="C79" s="10" t="n"/>
-      <c r="D79" s="10" t="n"/>
-      <c r="E79" s="10" t="n"/>
-      <c r="F79" s="11" t="n"/>
       <c r="G79" s="5" t="n"/>
       <c r="H79" s="5" t="n"/>
       <c r="I79" s="5" t="n"/>
@@ -1605,14 +1235,6 @@
           <t>DEMANDAS AMBIENTALES Y ESFUERZO FÍSICO</t>
         </is>
       </c>
-      <c r="B80" s="10" t="n"/>
-      <c r="C80" s="10" t="n"/>
-      <c r="D80" s="10" t="n"/>
-      <c r="E80" s="10" t="n"/>
-      <c r="F80" s="10" t="n"/>
-      <c r="G80" s="10" t="n"/>
-      <c r="H80" s="10" t="n"/>
-      <c r="I80" s="11" t="n"/>
     </row>
     <row r="81" ht="20" customHeight="1">
       <c r="A81" s="6" t="inlineStr">
@@ -1620,11 +1242,6 @@
           <t xml:space="preserve">   Item 1</t>
         </is>
       </c>
-      <c r="B81" s="10" t="n"/>
-      <c r="C81" s="10" t="n"/>
-      <c r="D81" s="10" t="n"/>
-      <c r="E81" s="10" t="n"/>
-      <c r="F81" s="11" t="n"/>
       <c r="G81" s="5" t="n"/>
       <c r="H81" s="5" t="n"/>
       <c r="I81" s="5" t="n"/>
@@ -1635,11 +1252,6 @@
           <t xml:space="preserve">   Item 2</t>
         </is>
       </c>
-      <c r="B82" s="10" t="n"/>
-      <c r="C82" s="10" t="n"/>
-      <c r="D82" s="10" t="n"/>
-      <c r="E82" s="10" t="n"/>
-      <c r="F82" s="11" t="n"/>
       <c r="G82" s="5" t="n"/>
       <c r="H82" s="5" t="n"/>
       <c r="I82" s="5" t="n"/>
@@ -1650,11 +1262,6 @@
           <t xml:space="preserve">   Item 3</t>
         </is>
       </c>
-      <c r="B83" s="10" t="n"/>
-      <c r="C83" s="10" t="n"/>
-      <c r="D83" s="10" t="n"/>
-      <c r="E83" s="10" t="n"/>
-      <c r="F83" s="11" t="n"/>
       <c r="G83" s="5" t="n"/>
       <c r="H83" s="5" t="n"/>
       <c r="I83" s="5" t="n"/>
@@ -1665,11 +1272,6 @@
           <t xml:space="preserve">   Item 4</t>
         </is>
       </c>
-      <c r="B84" s="10" t="n"/>
-      <c r="C84" s="10" t="n"/>
-      <c r="D84" s="10" t="n"/>
-      <c r="E84" s="10" t="n"/>
-      <c r="F84" s="11" t="n"/>
       <c r="G84" s="5" t="n"/>
       <c r="H84" s="5" t="n"/>
       <c r="I84" s="5" t="n"/>
@@ -1680,11 +1282,6 @@
           <t xml:space="preserve">   Item 5</t>
         </is>
       </c>
-      <c r="B85" s="10" t="n"/>
-      <c r="C85" s="10" t="n"/>
-      <c r="D85" s="10" t="n"/>
-      <c r="E85" s="10" t="n"/>
-      <c r="F85" s="11" t="n"/>
       <c r="G85" s="5" t="n"/>
       <c r="H85" s="5" t="n"/>
       <c r="I85" s="5" t="n"/>
@@ -1695,11 +1292,6 @@
           <t xml:space="preserve">   Item 6</t>
         </is>
       </c>
-      <c r="B86" s="10" t="n"/>
-      <c r="C86" s="10" t="n"/>
-      <c r="D86" s="10" t="n"/>
-      <c r="E86" s="10" t="n"/>
-      <c r="F86" s="11" t="n"/>
       <c r="G86" s="5" t="n"/>
       <c r="H86" s="5" t="n"/>
       <c r="I86" s="5" t="n"/>
@@ -1710,11 +1302,6 @@
           <t xml:space="preserve">   Item 7</t>
         </is>
       </c>
-      <c r="B87" s="10" t="n"/>
-      <c r="C87" s="10" t="n"/>
-      <c r="D87" s="10" t="n"/>
-      <c r="E87" s="10" t="n"/>
-      <c r="F87" s="11" t="n"/>
       <c r="G87" s="5" t="n"/>
       <c r="H87" s="5" t="n"/>
       <c r="I87" s="5" t="n"/>
@@ -1725,11 +1312,6 @@
           <t xml:space="preserve">   Item 8</t>
         </is>
       </c>
-      <c r="B88" s="10" t="n"/>
-      <c r="C88" s="10" t="n"/>
-      <c r="D88" s="10" t="n"/>
-      <c r="E88" s="10" t="n"/>
-      <c r="F88" s="11" t="n"/>
       <c r="G88" s="5" t="n"/>
       <c r="H88" s="5" t="n"/>
       <c r="I88" s="5" t="n"/>
@@ -1740,11 +1322,6 @@
           <t xml:space="preserve">   Item 9</t>
         </is>
       </c>
-      <c r="B89" s="10" t="n"/>
-      <c r="C89" s="10" t="n"/>
-      <c r="D89" s="10" t="n"/>
-      <c r="E89" s="10" t="n"/>
-      <c r="F89" s="11" t="n"/>
       <c r="G89" s="5" t="n"/>
       <c r="H89" s="5" t="n"/>
       <c r="I89" s="5" t="n"/>
@@ -1755,11 +1332,6 @@
           <t xml:space="preserve">   Item 10</t>
         </is>
       </c>
-      <c r="B90" s="10" t="n"/>
-      <c r="C90" s="10" t="n"/>
-      <c r="D90" s="10" t="n"/>
-      <c r="E90" s="10" t="n"/>
-      <c r="F90" s="11" t="n"/>
       <c r="G90" s="5" t="n"/>
       <c r="H90" s="5" t="n"/>
       <c r="I90" s="5" t="n"/>
@@ -1770,11 +1342,6 @@
           <t xml:space="preserve">   Item 11</t>
         </is>
       </c>
-      <c r="B91" s="10" t="n"/>
-      <c r="C91" s="10" t="n"/>
-      <c r="D91" s="10" t="n"/>
-      <c r="E91" s="10" t="n"/>
-      <c r="F91" s="11" t="n"/>
       <c r="G91" s="5" t="n"/>
       <c r="H91" s="5" t="n"/>
       <c r="I91" s="5" t="n"/>
@@ -1785,11 +1352,6 @@
           <t xml:space="preserve">   Item 12</t>
         </is>
       </c>
-      <c r="B92" s="10" t="n"/>
-      <c r="C92" s="10" t="n"/>
-      <c r="D92" s="10" t="n"/>
-      <c r="E92" s="10" t="n"/>
-      <c r="F92" s="11" t="n"/>
       <c r="G92" s="5" t="n"/>
       <c r="H92" s="5" t="n"/>
       <c r="I92" s="5" t="n"/>
@@ -1800,11 +1362,6 @@
           <t xml:space="preserve">   Item 13</t>
         </is>
       </c>
-      <c r="B93" s="10" t="n"/>
-      <c r="C93" s="10" t="n"/>
-      <c r="D93" s="10" t="n"/>
-      <c r="E93" s="10" t="n"/>
-      <c r="F93" s="11" t="n"/>
       <c r="G93" s="5" t="n"/>
       <c r="H93" s="5" t="n"/>
       <c r="I93" s="5" t="n"/>
@@ -1815,11 +1372,6 @@
           <t xml:space="preserve">   Item 14</t>
         </is>
       </c>
-      <c r="B94" s="10" t="n"/>
-      <c r="C94" s="10" t="n"/>
-      <c r="D94" s="10" t="n"/>
-      <c r="E94" s="10" t="n"/>
-      <c r="F94" s="11" t="n"/>
       <c r="G94" s="5" t="n"/>
       <c r="H94" s="5" t="n"/>
       <c r="I94" s="5" t="n"/>
@@ -1830,14 +1382,6 @@
           <t>DEMANDAS DE JORNADA</t>
         </is>
       </c>
-      <c r="B95" s="10" t="n"/>
-      <c r="C95" s="10" t="n"/>
-      <c r="D95" s="10" t="n"/>
-      <c r="E95" s="10" t="n"/>
-      <c r="F95" s="10" t="n"/>
-      <c r="G95" s="10" t="n"/>
-      <c r="H95" s="10" t="n"/>
-      <c r="I95" s="11" t="n"/>
     </row>
     <row r="96" ht="20" customHeight="1">
       <c r="A96" s="6" t="inlineStr">
@@ -1845,11 +1389,6 @@
           <t xml:space="preserve">   Item 1</t>
         </is>
       </c>
-      <c r="B96" s="10" t="n"/>
-      <c r="C96" s="10" t="n"/>
-      <c r="D96" s="10" t="n"/>
-      <c r="E96" s="10" t="n"/>
-      <c r="F96" s="11" t="n"/>
       <c r="G96" s="5" t="n"/>
       <c r="H96" s="5" t="n"/>
       <c r="I96" s="5" t="n"/>
@@ -1860,11 +1399,6 @@
           <t xml:space="preserve">   Item 2</t>
         </is>
       </c>
-      <c r="B97" s="10" t="n"/>
-      <c r="C97" s="10" t="n"/>
-      <c r="D97" s="10" t="n"/>
-      <c r="E97" s="10" t="n"/>
-      <c r="F97" s="11" t="n"/>
       <c r="G97" s="5" t="n"/>
       <c r="H97" s="5" t="n"/>
       <c r="I97" s="5" t="n"/>
@@ -1875,11 +1409,6 @@
           <t xml:space="preserve">   Item 3</t>
         </is>
       </c>
-      <c r="B98" s="10" t="n"/>
-      <c r="C98" s="10" t="n"/>
-      <c r="D98" s="10" t="n"/>
-      <c r="E98" s="10" t="n"/>
-      <c r="F98" s="11" t="n"/>
       <c r="G98" s="5" t="n"/>
       <c r="H98" s="5" t="n"/>
       <c r="I98" s="5" t="n"/>
@@ -1890,11 +1419,6 @@
           <t xml:space="preserve">   Item 4</t>
         </is>
       </c>
-      <c r="B99" s="10" t="n"/>
-      <c r="C99" s="10" t="n"/>
-      <c r="D99" s="10" t="n"/>
-      <c r="E99" s="10" t="n"/>
-      <c r="F99" s="11" t="n"/>
       <c r="G99" s="5" t="n"/>
       <c r="H99" s="5" t="n"/>
       <c r="I99" s="5" t="n"/>
@@ -1913,13 +1437,6 @@
         </is>
       </c>
       <c r="B102" s="6" t="n"/>
-      <c r="C102" s="10" t="n"/>
-      <c r="D102" s="10" t="n"/>
-      <c r="E102" s="10" t="n"/>
-      <c r="F102" s="10" t="n"/>
-      <c r="G102" s="10" t="n"/>
-      <c r="H102" s="10" t="n"/>
-      <c r="I102" s="11" t="n"/>
     </row>
     <row r="103" ht="30" customHeight="1">
       <c r="A103" s="4" t="inlineStr">
@@ -1928,13 +1445,6 @@
         </is>
       </c>
       <c r="B103" s="6" t="n"/>
-      <c r="C103" s="10" t="n"/>
-      <c r="D103" s="10" t="n"/>
-      <c r="E103" s="10" t="n"/>
-      <c r="F103" s="10" t="n"/>
-      <c r="G103" s="10" t="n"/>
-      <c r="H103" s="10" t="n"/>
-      <c r="I103" s="11" t="n"/>
     </row>
     <row r="104" ht="60" customHeight="1">
       <c r="A104" s="4" t="inlineStr">
@@ -1943,13 +1453,6 @@
         </is>
       </c>
       <c r="B104" s="6" t="n"/>
-      <c r="C104" s="10" t="n"/>
-      <c r="D104" s="10" t="n"/>
-      <c r="E104" s="10" t="n"/>
-      <c r="F104" s="10" t="n"/>
-      <c r="G104" s="10" t="n"/>
-      <c r="H104" s="10" t="n"/>
-      <c r="I104" s="11" t="n"/>
     </row>
     <row r="105" ht="60" customHeight="1">
       <c r="A105" s="4" t="inlineStr">
@@ -1958,13 +1461,6 @@
         </is>
       </c>
       <c r="B105" s="6" t="n"/>
-      <c r="C105" s="10" t="n"/>
-      <c r="D105" s="10" t="n"/>
-      <c r="E105" s="10" t="n"/>
-      <c r="F105" s="10" t="n"/>
-      <c r="G105" s="10" t="n"/>
-      <c r="H105" s="10" t="n"/>
-      <c r="I105" s="11" t="n"/>
     </row>
     <row r="107">
       <c r="A107" s="2" t="inlineStr">
@@ -1973,9 +1469,6 @@
         </is>
       </c>
       <c r="B107" s="5" t="n"/>
-      <c r="C107" s="10" t="n"/>
-      <c r="D107" s="10" t="n"/>
-      <c r="E107" s="11" t="n"/>
     </row>
     <row r="108">
       <c r="A108" s="2" t="inlineStr">
@@ -1984,9 +1477,6 @@
         </is>
       </c>
       <c r="B108" s="5" t="n"/>
-      <c r="C108" s="10" t="n"/>
-      <c r="D108" s="10" t="n"/>
-      <c r="E108" s="11" t="n"/>
     </row>
     <row r="109">
       <c r="A109" s="2" t="inlineStr">

</xml_diff>